<commit_message>
Major cleanup and reorganization after initial commit
</commit_message>
<xml_diff>
--- a/Dendro_data_supporting/Tomst_install.xlsx
+++ b/Dendro_data_supporting/Tomst_install.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/Dendrometers/Dendro_data_supporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Dendrometers/Dendro_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{98E03C99-2F99-44D8-9D25-7388A4E8D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE5C4F3D-04DF-4117-975A-D4361EFD39F7}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{98E03C99-2F99-44D8-9D25-7388A4E8D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F24CEBE7-5E9D-4904-9BCA-50577F0D547B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{937AFFAC-D172-4152-98E4-CB2C6927A2FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>TreeID</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Original one</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>2023-01-25 00:00:00</t>
   </si>
   <si>
@@ -203,12 +200,6 @@
     <t>????</t>
   </si>
   <si>
-    <t>Not needed- fig</t>
-  </si>
-  <si>
-    <t>Not needed- original is close enough</t>
-  </si>
-  <si>
     <t>Upper- near SF probes (?)</t>
   </si>
   <si>
@@ -246,6 +237,9 @@
   </si>
   <si>
     <t>2023-03-24 00:00:00</t>
+  </si>
+  <si>
+    <t>Original one, near SF sensors</t>
   </si>
 </sst>
 </file>
@@ -267,18 +261,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -299,13 +287,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AB57D3-2FAC-4042-A7C1-B1769EFDC3CD}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +635,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -659,37 +645,42 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2, B2)</f>
-        <v>ET1</v>
+        <v>ET1a</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>_xlfn.CONCAT(A3, B3)</f>
-        <v>ET1b</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C29" si="0">_xlfn.CONCAT(A3, B3)</f>
+        <v>ET2a</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,737 +688,537 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C41" si="0">_xlfn.CONCAT(A4, B4)</f>
-        <v>ET2a</v>
+        <f t="shared" si="0"/>
+        <v>ET2b</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>ET2b</v>
+        <v>ET3a</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>ET3</v>
+        <v>ET4a</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ET3b</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>56</v>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>ET4b</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>ET4a</v>
+        <v>ET5a</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>ET4b</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ET5b</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>ET5</v>
+        <v>ET6a</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ET5b</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
-        <v>54</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>ET7a</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>ET6a</v>
+        <v>ET8a</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ET6b</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2" t="s">
-        <v>55</v>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>FB1a</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>ET7</v>
+        <v>FB2a</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ET7b</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2" t="s">
-        <v>56</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>FB3a</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>ET8</v>
+        <v>FB3b</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ET8b</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>FB4a</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>FB1</v>
+        <v>FB4b</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>FB1b</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>FB5a</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>FB2</v>
+        <v>FB5b</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>FB6a</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>FB2b</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2" t="s">
-        <v>55</v>
+      <c r="F21" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>FB3a</v>
+        <v>FB6b</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>FB3b</v>
+        <v>FB7a</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>FB4a</v>
+        <v>FB7b</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>FB4b</v>
+        <v>FB8a</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>FB5a</v>
+        <v>TV1a</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>FB5b</v>
+        <v>TV2a</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>FB6a</v>
+        <v>TV3a</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>FB6b</v>
+        <v>TV4a</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>FB7a</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>FB7b</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>FB8</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>FB8b</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>TV1</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>TV1b</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>TV2</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>TV2b</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v>TV3</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>TV3b</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v>TV4a</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>TV4b</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>